<commit_message>
Updated Data Files and Main Code_10-7-25-11.05am
</commit_message>
<xml_diff>
--- a/Lab 3 Data/Excel Files/RWHEEL_T0pt2_Test.xlsx
+++ b/Lab 3 Data/Excel Files/RWHEEL_T0pt2_Test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Documents/GitHub Repositories/ASEN-3801-Lab-3/Lab 3 Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Documents/GitHub Repositories/ASEN-3801-Lab-3/Lab 3 Data/Excel Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24D8399B-0809-F040-8519-7397B1197A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F030C935-72E7-BF42-9006-A498FAAA19B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{91717659-3778-DF40-8A6B-2E288CD57104}"/>
+    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{CC2B1CAA-E3BE-FD46-91AF-CB6D3525821C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{6C9293D0-541F-314F-8936-59C60BA7106D}" name="RWHEEL_T0pt2_Test" type="6" refreshedVersion="8" background="1" saveData="1">
+  <connection id="1" xr16:uid="{3EDA477B-6ACE-2647-A883-E84D0A05CAD3}" name="RWHEEL_T0pt2_Test" type="6" refreshedVersion="8" background="1" saveData="1">
     <textPr codePage="10000" sourceFile="/Users/andrew/Documents/GitHub Repositories/ASEN-3801-Lab-3/Lab 3 Data/RWHEEL_T0pt2_Test.csv">
       <textFields count="5">
         <textField/>
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="RWHEEL_T0pt2_Test" connectionId="1" xr16:uid="{18B02210-3DB6-6A43-A2BE-E5E1F409DB98}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="RWHEEL_T0pt2_Test" connectionId="1" xr16:uid="{CA1A4894-E175-704A-AB8B-8EBC85BB8A15}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E0B4116-1FB1-F94C-B6DE-56B4B3E252D0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5BBE24-1B4D-F04F-ABB8-01E0233AF7A5}">
   <dimension ref="A1:E703"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>